<commit_message>
updating chart and read me files
</commit_message>
<xml_diff>
--- a/Gant Chart.xlsx
+++ b/Gant Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA90322A-FC05-C041-B9A9-3FD27C02DAA7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E247424E-728C-234A-BFD6-03051F3A2583}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
-  <si>
-    <t>Phase 1 Title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
   <si>
     <t>Task 3</t>
   </si>
@@ -150,9 +147,6 @@
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
   <si>
     <t>Sample phase title block</t>
@@ -228,10 +222,37 @@
 Repeat the instructions from cells A8 and A9 whenever you need to.</t>
   </si>
   <si>
-    <t xml:space="preserve">TBH </t>
-  </si>
-  <si>
     <t>Team B</t>
+  </si>
+  <si>
+    <t>Greg</t>
+  </si>
+  <si>
+    <t>Requirement gatherings</t>
+  </si>
+  <si>
+    <t>Business Rules</t>
+  </si>
+  <si>
+    <t>ERD Diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Megha </t>
+  </si>
+  <si>
+    <t>Megha &amp; Dannie</t>
+  </si>
+  <si>
+    <t>Building out the dbms</t>
+  </si>
+  <si>
+    <t>TBH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-commerce Website </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phase 1: Constructing the layout for the E-commerce Website </t>
   </si>
 </sst>
 </file>
@@ -642,7 +663,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -884,6 +905,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="12">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -891,17 +924,11 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1473,7 +1500,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1492,10 +1519,10 @@
   <sheetData>
     <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="59" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" s="63" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1503,386 +1530,386 @@
       <c r="F1" s="47"/>
       <c r="H1" s="2"/>
       <c r="I1" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="64" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I2" s="61" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="58" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="85" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="86"/>
-      <c r="E3" s="91">
+        <v>30</v>
+      </c>
+      <c r="C3" s="89" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="90"/>
+      <c r="E3" s="88">
         <f ca="1">TODAY()</f>
-        <v>43546</v>
-      </c>
-      <c r="F3" s="91"/>
+        <v>43551</v>
+      </c>
+      <c r="F3" s="88"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="59" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="85" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="86"/>
+        <v>41</v>
+      </c>
+      <c r="C4" s="89" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="90"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="88">
+      <c r="I4" s="85">
         <f ca="1">I5</f>
-        <v>43542</v>
-      </c>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="88">
+        <v>43549</v>
+      </c>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="85">
         <f ca="1">P5</f>
-        <v>43549</v>
-      </c>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="88">
+        <v>43556</v>
+      </c>
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="86"/>
+      <c r="V4" s="87"/>
+      <c r="W4" s="85">
         <f ca="1">W5</f>
-        <v>43556</v>
-      </c>
-      <c r="X4" s="89"/>
-      <c r="Y4" s="89"/>
-      <c r="Z4" s="89"/>
-      <c r="AA4" s="89"/>
-      <c r="AB4" s="89"/>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="88">
+        <v>43563</v>
+      </c>
+      <c r="X4" s="86"/>
+      <c r="Y4" s="86"/>
+      <c r="Z4" s="86"/>
+      <c r="AA4" s="86"/>
+      <c r="AB4" s="86"/>
+      <c r="AC4" s="87"/>
+      <c r="AD4" s="85">
         <f ca="1">AD5</f>
-        <v>43563</v>
-      </c>
-      <c r="AE4" s="89"/>
-      <c r="AF4" s="89"/>
-      <c r="AG4" s="89"/>
-      <c r="AH4" s="89"/>
-      <c r="AI4" s="89"/>
-      <c r="AJ4" s="90"/>
-      <c r="AK4" s="88">
+        <v>43570</v>
+      </c>
+      <c r="AE4" s="86"/>
+      <c r="AF4" s="86"/>
+      <c r="AG4" s="86"/>
+      <c r="AH4" s="86"/>
+      <c r="AI4" s="86"/>
+      <c r="AJ4" s="87"/>
+      <c r="AK4" s="85">
         <f ca="1">AK5</f>
-        <v>43570</v>
-      </c>
-      <c r="AL4" s="89"/>
-      <c r="AM4" s="89"/>
-      <c r="AN4" s="89"/>
-      <c r="AO4" s="89"/>
-      <c r="AP4" s="89"/>
-      <c r="AQ4" s="90"/>
-      <c r="AR4" s="88">
+        <v>43577</v>
+      </c>
+      <c r="AL4" s="86"/>
+      <c r="AM4" s="86"/>
+      <c r="AN4" s="86"/>
+      <c r="AO4" s="86"/>
+      <c r="AP4" s="86"/>
+      <c r="AQ4" s="87"/>
+      <c r="AR4" s="85">
         <f ca="1">AR5</f>
-        <v>43577</v>
-      </c>
-      <c r="AS4" s="89"/>
-      <c r="AT4" s="89"/>
-      <c r="AU4" s="89"/>
-      <c r="AV4" s="89"/>
-      <c r="AW4" s="89"/>
-      <c r="AX4" s="90"/>
-      <c r="AY4" s="88">
+        <v>43584</v>
+      </c>
+      <c r="AS4" s="86"/>
+      <c r="AT4" s="86"/>
+      <c r="AU4" s="86"/>
+      <c r="AV4" s="86"/>
+      <c r="AW4" s="86"/>
+      <c r="AX4" s="87"/>
+      <c r="AY4" s="85">
         <f ca="1">AY5</f>
-        <v>43584</v>
-      </c>
-      <c r="AZ4" s="89"/>
-      <c r="BA4" s="89"/>
-      <c r="BB4" s="89"/>
-      <c r="BC4" s="89"/>
-      <c r="BD4" s="89"/>
-      <c r="BE4" s="90"/>
-      <c r="BF4" s="88">
+        <v>43591</v>
+      </c>
+      <c r="AZ4" s="86"/>
+      <c r="BA4" s="86"/>
+      <c r="BB4" s="86"/>
+      <c r="BC4" s="86"/>
+      <c r="BD4" s="86"/>
+      <c r="BE4" s="87"/>
+      <c r="BF4" s="85">
         <f ca="1">BF5</f>
-        <v>43591</v>
-      </c>
-      <c r="BG4" s="89"/>
-      <c r="BH4" s="89"/>
-      <c r="BI4" s="89"/>
-      <c r="BJ4" s="89"/>
-      <c r="BK4" s="89"/>
-      <c r="BL4" s="90"/>
+        <v>43598</v>
+      </c>
+      <c r="BG4" s="86"/>
+      <c r="BH4" s="86"/>
+      <c r="BI4" s="86"/>
+      <c r="BJ4" s="86"/>
+      <c r="BK4" s="86"/>
+      <c r="BL4" s="87"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="59" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
+        <v>42</v>
+      </c>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>43542</v>
+        <v>43549</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">I5+1</f>
-        <v>43543</v>
+        <v>43550</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>43544</v>
+        <v>43551</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43545</v>
+        <v>43552</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43546</v>
+        <v>43553</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43547</v>
+        <v>43554</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43548</v>
+        <v>43555</v>
       </c>
       <c r="P5" s="11">
         <f ca="1">O5+1</f>
-        <v>43549</v>
+        <v>43556</v>
       </c>
       <c r="Q5" s="10">
         <f ca="1">P5+1</f>
-        <v>43550</v>
+        <v>43557</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43551</v>
+        <v>43558</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43552</v>
+        <v>43559</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43553</v>
+        <v>43560</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43554</v>
+        <v>43561</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43555</v>
+        <v>43562</v>
       </c>
       <c r="W5" s="11">
         <f ca="1">V5+1</f>
-        <v>43556</v>
+        <v>43563</v>
       </c>
       <c r="X5" s="10">
         <f ca="1">W5+1</f>
-        <v>43557</v>
+        <v>43564</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43558</v>
+        <v>43565</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43559</v>
+        <v>43566</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43560</v>
+        <v>43567</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43561</v>
+        <v>43568</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43562</v>
+        <v>43569</v>
       </c>
       <c r="AD5" s="11">
         <f ca="1">AC5+1</f>
-        <v>43563</v>
+        <v>43570</v>
       </c>
       <c r="AE5" s="10">
         <f ca="1">AD5+1</f>
-        <v>43564</v>
+        <v>43571</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43565</v>
+        <v>43572</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43566</v>
+        <v>43573</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43567</v>
+        <v>43574</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43568</v>
+        <v>43575</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43569</v>
+        <v>43576</v>
       </c>
       <c r="AK5" s="11">
         <f ca="1">AJ5+1</f>
-        <v>43570</v>
+        <v>43577</v>
       </c>
       <c r="AL5" s="10">
         <f ca="1">AK5+1</f>
-        <v>43571</v>
+        <v>43578</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43572</v>
+        <v>43579</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43573</v>
+        <v>43580</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43574</v>
+        <v>43581</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43575</v>
+        <v>43582</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43576</v>
+        <v>43583</v>
       </c>
       <c r="AR5" s="11">
         <f ca="1">AQ5+1</f>
-        <v>43577</v>
+        <v>43584</v>
       </c>
       <c r="AS5" s="10">
         <f ca="1">AR5+1</f>
-        <v>43578</v>
+        <v>43585</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43579</v>
+        <v>43586</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43580</v>
+        <v>43587</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43581</v>
+        <v>43588</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43582</v>
+        <v>43589</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43583</v>
+        <v>43590</v>
       </c>
       <c r="AY5" s="11">
         <f ca="1">AX5+1</f>
-        <v>43584</v>
+        <v>43591</v>
       </c>
       <c r="AZ5" s="10">
         <f ca="1">AY5+1</f>
-        <v>43585</v>
+        <v>43592</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>43586</v>
+        <v>43593</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>43587</v>
+        <v>43594</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>43588</v>
+        <v>43595</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>43589</v>
+        <v>43596</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" ca="1" si="1"/>
-        <v>43590</v>
+        <v>43597</v>
       </c>
       <c r="BF5" s="11">
         <f ca="1">BE5+1</f>
-        <v>43591</v>
+        <v>43598</v>
       </c>
       <c r="BG5" s="10">
         <f ca="1">BF5+1</f>
-        <v>43592</v>
+        <v>43599</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>43593</v>
+        <v>43600</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>43594</v>
+        <v>43601</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>43595</v>
+        <v>43602</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>43596</v>
+        <v>43603</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" ca="1" si="2"/>
-        <v>43597</v>
+        <v>43604</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>13</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="13" t="str">
         <f t="shared" ref="I6" ca="1" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
@@ -2111,7 +2138,7 @@
     </row>
     <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" s="62"/>
       <c r="E7"/>
@@ -2178,10 +2205,10 @@
     </row>
     <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="C8" s="71"/>
       <c r="D8" s="19"/>
@@ -2251,29 +2278,26 @@
     </row>
     <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="59" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="80" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="72" t="s">
-        <v>36</v>
+        <v>45</v>
+      </c>
+      <c r="B9" s="93" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="92" t="s">
+        <v>49</v>
       </c>
       <c r="D9" s="22">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E9" s="66">
         <f ca="1">Project_Start</f>
-        <v>43546</v>
-      </c>
-      <c r="F9" s="66">
-        <f ca="1">E9+3</f>
-        <v>43549</v>
-      </c>
+        <v>43551</v>
+      </c>
+      <c r="F9" s="66"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="17">
+      <c r="H9" s="17" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="I9" s="44"/>
       <c r="J9" s="44"/>
@@ -2334,27 +2358,25 @@
     </row>
     <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="59" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="80" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="72"/>
+        <v>46</v>
+      </c>
+      <c r="B10" s="93" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="92" t="s">
+        <v>53</v>
+      </c>
       <c r="D10" s="22">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="E10" s="66">
-        <f ca="1">F9</f>
-        <v>43549</v>
-      </c>
-      <c r="F10" s="66">
-        <f ca="1">E10+2</f>
         <v>43551</v>
       </c>
+      <c r="F10" s="66"/>
       <c r="G10" s="17"/>
-      <c r="H10" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+      <c r="H10" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="I10" s="44"/>
       <c r="J10" s="44"/>
@@ -2415,25 +2437,21 @@
     </row>
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="58"/>
-      <c r="B11" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="72"/>
+      <c r="B11" s="93" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="92" t="s">
+        <v>54</v>
+      </c>
       <c r="D11" s="22">
-        <v>0.5</v>
-      </c>
-      <c r="E11" s="66">
-        <f ca="1">F10</f>
-        <v>43551</v>
-      </c>
-      <c r="F11" s="66">
-        <f ca="1">E11+4</f>
-        <v>43555</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
       <c r="G11" s="17"/>
-      <c r="H11" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+      <c r="H11" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="I11" s="44"/>
       <c r="J11" s="44"/>
@@ -2494,25 +2512,21 @@
     </row>
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="58"/>
-      <c r="B12" s="80" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="72"/>
+      <c r="B12" s="93" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="92" t="s">
+        <v>56</v>
+      </c>
       <c r="D12" s="22">
-        <v>0.25</v>
-      </c>
-      <c r="E12" s="66">
-        <f ca="1">F11</f>
-        <v>43555</v>
-      </c>
-      <c r="F12" s="66">
-        <f ca="1">E12+5</f>
-        <v>43560</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
       <c r="G12" s="17"/>
-      <c r="H12" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>6</v>
+      <c r="H12" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="I12" s="44"/>
       <c r="J12" s="44"/>
@@ -2574,22 +2588,16 @@
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="58"/>
       <c r="B13" s="80" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="72"/>
       <c r="D13" s="22"/>
-      <c r="E13" s="66">
-        <f ca="1">E10+1</f>
-        <v>43550</v>
-      </c>
-      <c r="F13" s="66">
-        <f ca="1">E13+2</f>
-        <v>43552</v>
-      </c>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
       <c r="G13" s="17"/>
-      <c r="H13" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+      <c r="H13" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="I13" s="44"/>
       <c r="J13" s="44"/>
@@ -2650,10 +2658,10 @@
     </row>
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="59" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="73"/>
       <c r="D14" s="24"/>
@@ -2724,24 +2732,16 @@
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="59"/>
       <c r="B15" s="81" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="74"/>
-      <c r="D15" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="E15" s="67">
-        <f ca="1">E13+1</f>
-        <v>43551</v>
-      </c>
-      <c r="F15" s="67">
-        <f ca="1">E15+4</f>
-        <v>43555</v>
-      </c>
+      <c r="D15" s="27"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
       <c r="G15" s="17"/>
-      <c r="H15" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+      <c r="H15" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="I15" s="44"/>
       <c r="J15" s="44"/>
@@ -2803,24 +2803,16 @@
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="58"/>
       <c r="B16" s="81" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="74"/>
-      <c r="D16" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="E16" s="67">
-        <f ca="1">E15+2</f>
-        <v>43553</v>
-      </c>
-      <c r="F16" s="67">
-        <f ca="1">E16+5</f>
-        <v>43558</v>
-      </c>
+      <c r="D16" s="27"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
       <c r="G16" s="17"/>
-      <c r="H16" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>6</v>
+      <c r="H16" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="I16" s="44"/>
       <c r="J16" s="44"/>
@@ -2882,22 +2874,16 @@
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="58"/>
       <c r="B17" s="81" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="74"/>
       <c r="D17" s="27"/>
-      <c r="E17" s="67">
-        <f ca="1">F16</f>
-        <v>43558</v>
-      </c>
-      <c r="F17" s="67">
-        <f ca="1">E17+3</f>
-        <v>43561</v>
-      </c>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
       <c r="G17" s="17"/>
-      <c r="H17" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+      <c r="H17" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="I17" s="44"/>
       <c r="J17" s="44"/>
@@ -2959,22 +2945,16 @@
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="58"/>
       <c r="B18" s="81" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="74"/>
       <c r="D18" s="27"/>
-      <c r="E18" s="67">
-        <f ca="1">E17</f>
-        <v>43558</v>
-      </c>
-      <c r="F18" s="67">
-        <f ca="1">E18+2</f>
-        <v>43560</v>
-      </c>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
       <c r="G18" s="17"/>
-      <c r="H18" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+      <c r="H18" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="I18" s="44"/>
       <c r="J18" s="44"/>
@@ -3036,22 +3016,16 @@
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="58"/>
       <c r="B19" s="81" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="74"/>
       <c r="D19" s="27"/>
-      <c r="E19" s="67">
-        <f ca="1">E18</f>
-        <v>43558</v>
-      </c>
-      <c r="F19" s="67">
-        <f ca="1">E19+3</f>
-        <v>43561</v>
-      </c>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
       <c r="G19" s="17"/>
-      <c r="H19" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+      <c r="H19" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="I19" s="44"/>
       <c r="J19" s="44"/>
@@ -3112,10 +3086,10 @@
     </row>
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="58" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="75"/>
       <c r="D20" s="29"/>
@@ -3186,17 +3160,17 @@
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="58"/>
       <c r="B21" s="82" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="76"/>
       <c r="D21" s="32"/>
       <c r="E21" s="68">
         <f ca="1">E9+15</f>
-        <v>43561</v>
+        <v>43566</v>
       </c>
       <c r="F21" s="68">
         <f ca="1">E21+5</f>
-        <v>43566</v>
+        <v>43571</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17">
@@ -3263,17 +3237,17 @@
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="58"/>
       <c r="B22" s="82" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="76"/>
       <c r="D22" s="32"/>
       <c r="E22" s="68">
         <f ca="1">F21+1</f>
-        <v>43567</v>
+        <v>43572</v>
       </c>
       <c r="F22" s="68">
         <f ca="1">E22+4</f>
-        <v>43571</v>
+        <v>43576</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17">
@@ -3340,17 +3314,17 @@
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="58"/>
       <c r="B23" s="82" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="76"/>
       <c r="D23" s="32"/>
       <c r="E23" s="68">
         <f ca="1">E22+5</f>
-        <v>43572</v>
+        <v>43577</v>
       </c>
       <c r="F23" s="68">
         <f ca="1">E23+5</f>
-        <v>43577</v>
+        <v>43582</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17">
@@ -3417,17 +3391,17 @@
     <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="58"/>
       <c r="B24" s="82" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" s="76"/>
       <c r="D24" s="32"/>
       <c r="E24" s="68">
         <f ca="1">F23+1</f>
-        <v>43578</v>
+        <v>43583</v>
       </c>
       <c r="F24" s="68">
         <f ca="1">E24+4</f>
-        <v>43582</v>
+        <v>43587</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17">
@@ -3494,17 +3468,17 @@
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="58"/>
       <c r="B25" s="82" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" s="76"/>
       <c r="D25" s="32"/>
       <c r="E25" s="68">
         <f ca="1">E23</f>
-        <v>43572</v>
+        <v>43577</v>
       </c>
       <c r="F25" s="68">
         <f ca="1">E25+4</f>
-        <v>43576</v>
+        <v>43581</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="17">
@@ -3570,10 +3544,10 @@
     </row>
     <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="58" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="77"/>
       <c r="D26" s="34"/>
@@ -3644,15 +3618,15 @@
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="58"/>
       <c r="B27" s="83" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" s="78"/>
       <c r="D27" s="37"/>
       <c r="E27" s="69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F27" s="69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="17" t="e">
@@ -3719,15 +3693,15 @@
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="58"/>
       <c r="B28" s="83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" s="78"/>
       <c r="D28" s="37"/>
       <c r="E28" s="69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F28" s="69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="17" t="e">
@@ -3794,15 +3768,15 @@
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="58"/>
       <c r="B29" s="83" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" s="78"/>
       <c r="D29" s="37"/>
       <c r="E29" s="69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F29" s="69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="17" t="e">
@@ -3869,15 +3843,15 @@
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="58"/>
       <c r="B30" s="83" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" s="78"/>
       <c r="D30" s="37"/>
       <c r="E30" s="69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F30" s="69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="17" t="e">
@@ -3944,15 +3918,15 @@
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="58"/>
       <c r="B31" s="83" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31" s="78"/>
       <c r="D31" s="37"/>
       <c r="E31" s="69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F31" s="69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="17" t="e">
@@ -4018,7 +3992,7 @@
     </row>
     <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="58" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B32" s="84"/>
       <c r="C32" s="79"/>
@@ -4089,10 +4063,10 @@
     </row>
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="59" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" s="39"/>
       <c r="D33" s="40"/>
@@ -4172,6 +4146,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4179,11 +4158,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">
@@ -4228,7 +4202,7 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="F18 F22:F23 E23" formula="1"/>
+    <ignoredError sqref="F22:F23 E23" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -4269,79 +4243,79 @@
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:2" s="50" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="49"/>
     </row>
     <row r="3" spans="1:2" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="55"/>
     </row>
     <row r="4" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="74" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="48" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="57" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A8" s="52" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="53" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="48" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A11" s="52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="48" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A14" s="52" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="53" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated gant chart and readme
</commit_message>
<xml_diff>
--- a/Gant Chart.xlsx
+++ b/Gant Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E247424E-728C-234A-BFD6-03051F3A2583}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7691ABB9-5E1D-4141-AE6E-9F77109510FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
   <si>
     <t>Task 3</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t xml:space="preserve">Phase 1: Constructing the layout for the E-commerce Website </t>
+  </si>
+  <si>
+    <t>Setup bootstrap</t>
   </si>
 </sst>
 </file>
@@ -663,7 +666,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -890,9 +893,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="11">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -905,6 +905,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="12">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -916,19 +929,6 @@
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1500,7 +1500,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1551,341 +1551,341 @@
       <c r="B3" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="89" t="s">
+      <c r="C3" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="90"/>
-      <c r="E3" s="88">
+      <c r="D3" s="87"/>
+      <c r="E3" s="92">
         <f ca="1">TODAY()</f>
-        <v>43551</v>
-      </c>
-      <c r="F3" s="88"/>
+        <v>43562</v>
+      </c>
+      <c r="F3" s="92"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="90"/>
+      <c r="D4" s="87"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="85">
+      <c r="I4" s="89">
         <f ca="1">I5</f>
-        <v>43549</v>
-      </c>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="85">
+        <v>43563</v>
+      </c>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="89">
         <f ca="1">P5</f>
-        <v>43556</v>
-      </c>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="85">
+        <v>43570</v>
+      </c>
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="91"/>
+      <c r="W4" s="89">
         <f ca="1">W5</f>
-        <v>43563</v>
-      </c>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="85">
+        <v>43577</v>
+      </c>
+      <c r="X4" s="90"/>
+      <c r="Y4" s="90"/>
+      <c r="Z4" s="90"/>
+      <c r="AA4" s="90"/>
+      <c r="AB4" s="90"/>
+      <c r="AC4" s="91"/>
+      <c r="AD4" s="89">
         <f ca="1">AD5</f>
-        <v>43570</v>
-      </c>
-      <c r="AE4" s="86"/>
-      <c r="AF4" s="86"/>
-      <c r="AG4" s="86"/>
-      <c r="AH4" s="86"/>
-      <c r="AI4" s="86"/>
-      <c r="AJ4" s="87"/>
-      <c r="AK4" s="85">
+        <v>43584</v>
+      </c>
+      <c r="AE4" s="90"/>
+      <c r="AF4" s="90"/>
+      <c r="AG4" s="90"/>
+      <c r="AH4" s="90"/>
+      <c r="AI4" s="90"/>
+      <c r="AJ4" s="91"/>
+      <c r="AK4" s="89">
         <f ca="1">AK5</f>
-        <v>43577</v>
-      </c>
-      <c r="AL4" s="86"/>
-      <c r="AM4" s="86"/>
-      <c r="AN4" s="86"/>
-      <c r="AO4" s="86"/>
-      <c r="AP4" s="86"/>
-      <c r="AQ4" s="87"/>
-      <c r="AR4" s="85">
+        <v>43591</v>
+      </c>
+      <c r="AL4" s="90"/>
+      <c r="AM4" s="90"/>
+      <c r="AN4" s="90"/>
+      <c r="AO4" s="90"/>
+      <c r="AP4" s="90"/>
+      <c r="AQ4" s="91"/>
+      <c r="AR4" s="89">
         <f ca="1">AR5</f>
-        <v>43584</v>
-      </c>
-      <c r="AS4" s="86"/>
-      <c r="AT4" s="86"/>
-      <c r="AU4" s="86"/>
-      <c r="AV4" s="86"/>
-      <c r="AW4" s="86"/>
-      <c r="AX4" s="87"/>
-      <c r="AY4" s="85">
+        <v>43598</v>
+      </c>
+      <c r="AS4" s="90"/>
+      <c r="AT4" s="90"/>
+      <c r="AU4" s="90"/>
+      <c r="AV4" s="90"/>
+      <c r="AW4" s="90"/>
+      <c r="AX4" s="91"/>
+      <c r="AY4" s="89">
         <f ca="1">AY5</f>
-        <v>43591</v>
-      </c>
-      <c r="AZ4" s="86"/>
-      <c r="BA4" s="86"/>
-      <c r="BB4" s="86"/>
-      <c r="BC4" s="86"/>
-      <c r="BD4" s="86"/>
-      <c r="BE4" s="87"/>
-      <c r="BF4" s="85">
+        <v>43605</v>
+      </c>
+      <c r="AZ4" s="90"/>
+      <c r="BA4" s="90"/>
+      <c r="BB4" s="90"/>
+      <c r="BC4" s="90"/>
+      <c r="BD4" s="90"/>
+      <c r="BE4" s="91"/>
+      <c r="BF4" s="89">
         <f ca="1">BF5</f>
-        <v>43598</v>
-      </c>
-      <c r="BG4" s="86"/>
-      <c r="BH4" s="86"/>
-      <c r="BI4" s="86"/>
-      <c r="BJ4" s="86"/>
-      <c r="BK4" s="86"/>
-      <c r="BL4" s="87"/>
+        <v>43612</v>
+      </c>
+      <c r="BG4" s="90"/>
+      <c r="BH4" s="90"/>
+      <c r="BI4" s="90"/>
+      <c r="BJ4" s="90"/>
+      <c r="BK4" s="90"/>
+      <c r="BL4" s="91"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>43549</v>
+        <v>43563</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">I5+1</f>
-        <v>43550</v>
+        <v>43564</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>43551</v>
+        <v>43565</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43552</v>
+        <v>43566</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43553</v>
+        <v>43567</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43554</v>
+        <v>43568</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43555</v>
+        <v>43569</v>
       </c>
       <c r="P5" s="11">
         <f ca="1">O5+1</f>
-        <v>43556</v>
+        <v>43570</v>
       </c>
       <c r="Q5" s="10">
         <f ca="1">P5+1</f>
-        <v>43557</v>
+        <v>43571</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43558</v>
+        <v>43572</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43559</v>
+        <v>43573</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43560</v>
+        <v>43574</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43561</v>
+        <v>43575</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43562</v>
+        <v>43576</v>
       </c>
       <c r="W5" s="11">
         <f ca="1">V5+1</f>
-        <v>43563</v>
+        <v>43577</v>
       </c>
       <c r="X5" s="10">
         <f ca="1">W5+1</f>
-        <v>43564</v>
+        <v>43578</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43565</v>
+        <v>43579</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43566</v>
+        <v>43580</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43567</v>
+        <v>43581</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43568</v>
+        <v>43582</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43569</v>
+        <v>43583</v>
       </c>
       <c r="AD5" s="11">
         <f ca="1">AC5+1</f>
-        <v>43570</v>
+        <v>43584</v>
       </c>
       <c r="AE5" s="10">
         <f ca="1">AD5+1</f>
-        <v>43571</v>
+        <v>43585</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43572</v>
+        <v>43586</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43573</v>
+        <v>43587</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43574</v>
+        <v>43588</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43575</v>
+        <v>43589</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43576</v>
+        <v>43590</v>
       </c>
       <c r="AK5" s="11">
         <f ca="1">AJ5+1</f>
-        <v>43577</v>
+        <v>43591</v>
       </c>
       <c r="AL5" s="10">
         <f ca="1">AK5+1</f>
-        <v>43578</v>
+        <v>43592</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43579</v>
+        <v>43593</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43580</v>
+        <v>43594</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43581</v>
+        <v>43595</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43582</v>
+        <v>43596</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43583</v>
+        <v>43597</v>
       </c>
       <c r="AR5" s="11">
         <f ca="1">AQ5+1</f>
-        <v>43584</v>
+        <v>43598</v>
       </c>
       <c r="AS5" s="10">
         <f ca="1">AR5+1</f>
-        <v>43585</v>
+        <v>43599</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43586</v>
+        <v>43600</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43587</v>
+        <v>43601</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43588</v>
+        <v>43602</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43589</v>
+        <v>43603</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43590</v>
+        <v>43604</v>
       </c>
       <c r="AY5" s="11">
         <f ca="1">AX5+1</f>
-        <v>43591</v>
+        <v>43605</v>
       </c>
       <c r="AZ5" s="10">
         <f ca="1">AY5+1</f>
-        <v>43592</v>
+        <v>43606</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>43593</v>
+        <v>43607</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>43594</v>
+        <v>43608</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>43595</v>
+        <v>43609</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>43596</v>
+        <v>43610</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" ca="1" si="1"/>
-        <v>43597</v>
+        <v>43611</v>
       </c>
       <c r="BF5" s="11">
         <f ca="1">BE5+1</f>
-        <v>43598</v>
+        <v>43612</v>
       </c>
       <c r="BG5" s="10">
         <f ca="1">BF5+1</f>
-        <v>43599</v>
+        <v>43613</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>43600</v>
+        <v>43614</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>43601</v>
+        <v>43615</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>43602</v>
+        <v>43616</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>43603</v>
+        <v>43617</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" ca="1" si="2"/>
-        <v>43604</v>
+        <v>43618</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2280,18 +2280,18 @@
       <c r="A9" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="93" t="s">
+      <c r="B9" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="92" t="s">
+      <c r="C9" s="84" t="s">
         <v>49</v>
       </c>
       <c r="D9" s="22">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E9" s="66">
         <f ca="1">Project_Start</f>
-        <v>43551</v>
+        <v>43562</v>
       </c>
       <c r="F9" s="66"/>
       <c r="G9" s="17"/>
@@ -2360,14 +2360,14 @@
       <c r="A10" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="93" t="s">
+      <c r="B10" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="92" t="s">
+      <c r="C10" s="84" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="22">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E10" s="66">
         <v>43551</v>
@@ -2437,10 +2437,10 @@
     </row>
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="58"/>
-      <c r="B11" s="93" t="s">
+      <c r="B11" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="92" t="s">
+      <c r="C11" s="84" t="s">
         <v>54</v>
       </c>
       <c r="D11" s="22">
@@ -2512,10 +2512,10 @@
     </row>
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="58"/>
-      <c r="B12" s="93" t="s">
+      <c r="B12" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="92" t="s">
+      <c r="C12" s="84" t="s">
         <v>56</v>
       </c>
       <c r="D12" s="22">
@@ -2587,8 +2587,8 @@
     </row>
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="58"/>
-      <c r="B13" s="80" t="s">
-        <v>2</v>
+      <c r="B13" s="85" t="s">
+        <v>59</v>
       </c>
       <c r="C13" s="72"/>
       <c r="D13" s="22"/>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="59"/>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="80" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="74"/>
@@ -2802,7 +2802,7 @@
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="58"/>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="80" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="74"/>
@@ -2873,7 +2873,7 @@
     </row>
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="58"/>
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="80" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="74"/>
@@ -2944,7 +2944,7 @@
     </row>
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="58"/>
-      <c r="B18" s="81" t="s">
+      <c r="B18" s="80" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="74"/>
@@ -3015,7 +3015,7 @@
     </row>
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="58"/>
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="80" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="74"/>
@@ -3159,18 +3159,18 @@
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="58"/>
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="81" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="76"/>
       <c r="D21" s="32"/>
       <c r="E21" s="68">
         <f ca="1">E9+15</f>
-        <v>43566</v>
+        <v>43577</v>
       </c>
       <c r="F21" s="68">
         <f ca="1">E21+5</f>
-        <v>43571</v>
+        <v>43582</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17">
@@ -3236,18 +3236,18 @@
     </row>
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="58"/>
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="81" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="76"/>
       <c r="D22" s="32"/>
       <c r="E22" s="68">
         <f ca="1">F21+1</f>
-        <v>43572</v>
+        <v>43583</v>
       </c>
       <c r="F22" s="68">
         <f ca="1">E22+4</f>
-        <v>43576</v>
+        <v>43587</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17">
@@ -3313,18 +3313,18 @@
     </row>
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="58"/>
-      <c r="B23" s="82" t="s">
+      <c r="B23" s="81" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="76"/>
       <c r="D23" s="32"/>
       <c r="E23" s="68">
         <f ca="1">E22+5</f>
-        <v>43577</v>
+        <v>43588</v>
       </c>
       <c r="F23" s="68">
         <f ca="1">E23+5</f>
-        <v>43582</v>
+        <v>43593</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17">
@@ -3390,18 +3390,18 @@
     </row>
     <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="58"/>
-      <c r="B24" s="82" t="s">
+      <c r="B24" s="81" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="76"/>
       <c r="D24" s="32"/>
       <c r="E24" s="68">
         <f ca="1">F23+1</f>
-        <v>43583</v>
+        <v>43594</v>
       </c>
       <c r="F24" s="68">
         <f ca="1">E24+4</f>
-        <v>43587</v>
+        <v>43598</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17">
@@ -3467,18 +3467,18 @@
     </row>
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="58"/>
-      <c r="B25" s="82" t="s">
+      <c r="B25" s="81" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="76"/>
       <c r="D25" s="32"/>
       <c r="E25" s="68">
         <f ca="1">E23</f>
-        <v>43577</v>
+        <v>43588</v>
       </c>
       <c r="F25" s="68">
         <f ca="1">E25+4</f>
-        <v>43581</v>
+        <v>43592</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="17">
@@ -3617,7 +3617,7 @@
     </row>
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="58"/>
-      <c r="B27" s="83" t="s">
+      <c r="B27" s="82" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="78"/>
@@ -3692,7 +3692,7 @@
     </row>
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="58"/>
-      <c r="B28" s="83" t="s">
+      <c r="B28" s="82" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="78"/>
@@ -3767,7 +3767,7 @@
     </row>
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="58"/>
-      <c r="B29" s="83" t="s">
+      <c r="B29" s="82" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="78"/>
@@ -3842,7 +3842,7 @@
     </row>
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="58"/>
-      <c r="B30" s="83" t="s">
+      <c r="B30" s="82" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="78"/>
@@ -3917,7 +3917,7 @@
     </row>
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="58"/>
-      <c r="B31" s="83" t="s">
+      <c r="B31" s="82" t="s">
         <v>2</v>
       </c>
       <c r="C31" s="78"/>
@@ -3994,7 +3994,7 @@
       <c r="A32" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="84"/>
+      <c r="B32" s="83"/>
       <c r="C32" s="79"/>
       <c r="D32" s="16"/>
       <c r="E32" s="70"/>
@@ -4146,11 +4146,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4158,6 +4153,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">

</xml_diff>

<commit_message>
ER diagram of ecommerce_website
</commit_message>
<xml_diff>
--- a/Gant Chart.xlsx
+++ b/Gant Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E247424E-728C-234A-BFD6-03051F3A2583}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7691ABB9-5E1D-4141-AE6E-9F77109510FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
   <si>
     <t>Task 3</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t xml:space="preserve">Phase 1: Constructing the layout for the E-commerce Website </t>
+  </si>
+  <si>
+    <t>Setup bootstrap</t>
   </si>
 </sst>
 </file>
@@ -663,7 +666,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -890,9 +893,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="11">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -905,6 +905,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="12">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -916,19 +929,6 @@
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1500,7 +1500,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1551,341 +1551,341 @@
       <c r="B3" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="89" t="s">
+      <c r="C3" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="90"/>
-      <c r="E3" s="88">
+      <c r="D3" s="87"/>
+      <c r="E3" s="92">
         <f ca="1">TODAY()</f>
-        <v>43551</v>
-      </c>
-      <c r="F3" s="88"/>
+        <v>43562</v>
+      </c>
+      <c r="F3" s="92"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="90"/>
+      <c r="D4" s="87"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="85">
+      <c r="I4" s="89">
         <f ca="1">I5</f>
-        <v>43549</v>
-      </c>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="85">
+        <v>43563</v>
+      </c>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="89">
         <f ca="1">P5</f>
-        <v>43556</v>
-      </c>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="85">
+        <v>43570</v>
+      </c>
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="91"/>
+      <c r="W4" s="89">
         <f ca="1">W5</f>
-        <v>43563</v>
-      </c>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="85">
+        <v>43577</v>
+      </c>
+      <c r="X4" s="90"/>
+      <c r="Y4" s="90"/>
+      <c r="Z4" s="90"/>
+      <c r="AA4" s="90"/>
+      <c r="AB4" s="90"/>
+      <c r="AC4" s="91"/>
+      <c r="AD4" s="89">
         <f ca="1">AD5</f>
-        <v>43570</v>
-      </c>
-      <c r="AE4" s="86"/>
-      <c r="AF4" s="86"/>
-      <c r="AG4" s="86"/>
-      <c r="AH4" s="86"/>
-      <c r="AI4" s="86"/>
-      <c r="AJ4" s="87"/>
-      <c r="AK4" s="85">
+        <v>43584</v>
+      </c>
+      <c r="AE4" s="90"/>
+      <c r="AF4" s="90"/>
+      <c r="AG4" s="90"/>
+      <c r="AH4" s="90"/>
+      <c r="AI4" s="90"/>
+      <c r="AJ4" s="91"/>
+      <c r="AK4" s="89">
         <f ca="1">AK5</f>
-        <v>43577</v>
-      </c>
-      <c r="AL4" s="86"/>
-      <c r="AM4" s="86"/>
-      <c r="AN4" s="86"/>
-      <c r="AO4" s="86"/>
-      <c r="AP4" s="86"/>
-      <c r="AQ4" s="87"/>
-      <c r="AR4" s="85">
+        <v>43591</v>
+      </c>
+      <c r="AL4" s="90"/>
+      <c r="AM4" s="90"/>
+      <c r="AN4" s="90"/>
+      <c r="AO4" s="90"/>
+      <c r="AP4" s="90"/>
+      <c r="AQ4" s="91"/>
+      <c r="AR4" s="89">
         <f ca="1">AR5</f>
-        <v>43584</v>
-      </c>
-      <c r="AS4" s="86"/>
-      <c r="AT4" s="86"/>
-      <c r="AU4" s="86"/>
-      <c r="AV4" s="86"/>
-      <c r="AW4" s="86"/>
-      <c r="AX4" s="87"/>
-      <c r="AY4" s="85">
+        <v>43598</v>
+      </c>
+      <c r="AS4" s="90"/>
+      <c r="AT4" s="90"/>
+      <c r="AU4" s="90"/>
+      <c r="AV4" s="90"/>
+      <c r="AW4" s="90"/>
+      <c r="AX4" s="91"/>
+      <c r="AY4" s="89">
         <f ca="1">AY5</f>
-        <v>43591</v>
-      </c>
-      <c r="AZ4" s="86"/>
-      <c r="BA4" s="86"/>
-      <c r="BB4" s="86"/>
-      <c r="BC4" s="86"/>
-      <c r="BD4" s="86"/>
-      <c r="BE4" s="87"/>
-      <c r="BF4" s="85">
+        <v>43605</v>
+      </c>
+      <c r="AZ4" s="90"/>
+      <c r="BA4" s="90"/>
+      <c r="BB4" s="90"/>
+      <c r="BC4" s="90"/>
+      <c r="BD4" s="90"/>
+      <c r="BE4" s="91"/>
+      <c r="BF4" s="89">
         <f ca="1">BF5</f>
-        <v>43598</v>
-      </c>
-      <c r="BG4" s="86"/>
-      <c r="BH4" s="86"/>
-      <c r="BI4" s="86"/>
-      <c r="BJ4" s="86"/>
-      <c r="BK4" s="86"/>
-      <c r="BL4" s="87"/>
+        <v>43612</v>
+      </c>
+      <c r="BG4" s="90"/>
+      <c r="BH4" s="90"/>
+      <c r="BI4" s="90"/>
+      <c r="BJ4" s="90"/>
+      <c r="BK4" s="90"/>
+      <c r="BL4" s="91"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>43549</v>
+        <v>43563</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">I5+1</f>
-        <v>43550</v>
+        <v>43564</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>43551</v>
+        <v>43565</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43552</v>
+        <v>43566</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43553</v>
+        <v>43567</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43554</v>
+        <v>43568</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43555</v>
+        <v>43569</v>
       </c>
       <c r="P5" s="11">
         <f ca="1">O5+1</f>
-        <v>43556</v>
+        <v>43570</v>
       </c>
       <c r="Q5" s="10">
         <f ca="1">P5+1</f>
-        <v>43557</v>
+        <v>43571</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43558</v>
+        <v>43572</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43559</v>
+        <v>43573</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43560</v>
+        <v>43574</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43561</v>
+        <v>43575</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43562</v>
+        <v>43576</v>
       </c>
       <c r="W5" s="11">
         <f ca="1">V5+1</f>
-        <v>43563</v>
+        <v>43577</v>
       </c>
       <c r="X5" s="10">
         <f ca="1">W5+1</f>
-        <v>43564</v>
+        <v>43578</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43565</v>
+        <v>43579</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43566</v>
+        <v>43580</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43567</v>
+        <v>43581</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43568</v>
+        <v>43582</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43569</v>
+        <v>43583</v>
       </c>
       <c r="AD5" s="11">
         <f ca="1">AC5+1</f>
-        <v>43570</v>
+        <v>43584</v>
       </c>
       <c r="AE5" s="10">
         <f ca="1">AD5+1</f>
-        <v>43571</v>
+        <v>43585</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43572</v>
+        <v>43586</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43573</v>
+        <v>43587</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43574</v>
+        <v>43588</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43575</v>
+        <v>43589</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43576</v>
+        <v>43590</v>
       </c>
       <c r="AK5" s="11">
         <f ca="1">AJ5+1</f>
-        <v>43577</v>
+        <v>43591</v>
       </c>
       <c r="AL5" s="10">
         <f ca="1">AK5+1</f>
-        <v>43578</v>
+        <v>43592</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43579</v>
+        <v>43593</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43580</v>
+        <v>43594</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43581</v>
+        <v>43595</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43582</v>
+        <v>43596</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43583</v>
+        <v>43597</v>
       </c>
       <c r="AR5" s="11">
         <f ca="1">AQ5+1</f>
-        <v>43584</v>
+        <v>43598</v>
       </c>
       <c r="AS5" s="10">
         <f ca="1">AR5+1</f>
-        <v>43585</v>
+        <v>43599</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43586</v>
+        <v>43600</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43587</v>
+        <v>43601</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43588</v>
+        <v>43602</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43589</v>
+        <v>43603</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43590</v>
+        <v>43604</v>
       </c>
       <c r="AY5" s="11">
         <f ca="1">AX5+1</f>
-        <v>43591</v>
+        <v>43605</v>
       </c>
       <c r="AZ5" s="10">
         <f ca="1">AY5+1</f>
-        <v>43592</v>
+        <v>43606</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>43593</v>
+        <v>43607</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>43594</v>
+        <v>43608</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>43595</v>
+        <v>43609</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>43596</v>
+        <v>43610</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" ca="1" si="1"/>
-        <v>43597</v>
+        <v>43611</v>
       </c>
       <c r="BF5" s="11">
         <f ca="1">BE5+1</f>
-        <v>43598</v>
+        <v>43612</v>
       </c>
       <c r="BG5" s="10">
         <f ca="1">BF5+1</f>
-        <v>43599</v>
+        <v>43613</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>43600</v>
+        <v>43614</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>43601</v>
+        <v>43615</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>43602</v>
+        <v>43616</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>43603</v>
+        <v>43617</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" ca="1" si="2"/>
-        <v>43604</v>
+        <v>43618</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2280,18 +2280,18 @@
       <c r="A9" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="93" t="s">
+      <c r="B9" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="92" t="s">
+      <c r="C9" s="84" t="s">
         <v>49</v>
       </c>
       <c r="D9" s="22">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E9" s="66">
         <f ca="1">Project_Start</f>
-        <v>43551</v>
+        <v>43562</v>
       </c>
       <c r="F9" s="66"/>
       <c r="G9" s="17"/>
@@ -2360,14 +2360,14 @@
       <c r="A10" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="93" t="s">
+      <c r="B10" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="92" t="s">
+      <c r="C10" s="84" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="22">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E10" s="66">
         <v>43551</v>
@@ -2437,10 +2437,10 @@
     </row>
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="58"/>
-      <c r="B11" s="93" t="s">
+      <c r="B11" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="92" t="s">
+      <c r="C11" s="84" t="s">
         <v>54</v>
       </c>
       <c r="D11" s="22">
@@ -2512,10 +2512,10 @@
     </row>
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="58"/>
-      <c r="B12" s="93" t="s">
+      <c r="B12" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="92" t="s">
+      <c r="C12" s="84" t="s">
         <v>56</v>
       </c>
       <c r="D12" s="22">
@@ -2587,8 +2587,8 @@
     </row>
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="58"/>
-      <c r="B13" s="80" t="s">
-        <v>2</v>
+      <c r="B13" s="85" t="s">
+        <v>59</v>
       </c>
       <c r="C13" s="72"/>
       <c r="D13" s="22"/>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="59"/>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="80" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="74"/>
@@ -2802,7 +2802,7 @@
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="58"/>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="80" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="74"/>
@@ -2873,7 +2873,7 @@
     </row>
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="58"/>
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="80" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="74"/>
@@ -2944,7 +2944,7 @@
     </row>
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="58"/>
-      <c r="B18" s="81" t="s">
+      <c r="B18" s="80" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="74"/>
@@ -3015,7 +3015,7 @@
     </row>
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="58"/>
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="80" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="74"/>
@@ -3159,18 +3159,18 @@
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="58"/>
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="81" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="76"/>
       <c r="D21" s="32"/>
       <c r="E21" s="68">
         <f ca="1">E9+15</f>
-        <v>43566</v>
+        <v>43577</v>
       </c>
       <c r="F21" s="68">
         <f ca="1">E21+5</f>
-        <v>43571</v>
+        <v>43582</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17">
@@ -3236,18 +3236,18 @@
     </row>
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="58"/>
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="81" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="76"/>
       <c r="D22" s="32"/>
       <c r="E22" s="68">
         <f ca="1">F21+1</f>
-        <v>43572</v>
+        <v>43583</v>
       </c>
       <c r="F22" s="68">
         <f ca="1">E22+4</f>
-        <v>43576</v>
+        <v>43587</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17">
@@ -3313,18 +3313,18 @@
     </row>
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="58"/>
-      <c r="B23" s="82" t="s">
+      <c r="B23" s="81" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="76"/>
       <c r="D23" s="32"/>
       <c r="E23" s="68">
         <f ca="1">E22+5</f>
-        <v>43577</v>
+        <v>43588</v>
       </c>
       <c r="F23" s="68">
         <f ca="1">E23+5</f>
-        <v>43582</v>
+        <v>43593</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17">
@@ -3390,18 +3390,18 @@
     </row>
     <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="58"/>
-      <c r="B24" s="82" t="s">
+      <c r="B24" s="81" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="76"/>
       <c r="D24" s="32"/>
       <c r="E24" s="68">
         <f ca="1">F23+1</f>
-        <v>43583</v>
+        <v>43594</v>
       </c>
       <c r="F24" s="68">
         <f ca="1">E24+4</f>
-        <v>43587</v>
+        <v>43598</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17">
@@ -3467,18 +3467,18 @@
     </row>
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="58"/>
-      <c r="B25" s="82" t="s">
+      <c r="B25" s="81" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="76"/>
       <c r="D25" s="32"/>
       <c r="E25" s="68">
         <f ca="1">E23</f>
-        <v>43577</v>
+        <v>43588</v>
       </c>
       <c r="F25" s="68">
         <f ca="1">E25+4</f>
-        <v>43581</v>
+        <v>43592</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="17">
@@ -3617,7 +3617,7 @@
     </row>
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="58"/>
-      <c r="B27" s="83" t="s">
+      <c r="B27" s="82" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="78"/>
@@ -3692,7 +3692,7 @@
     </row>
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="58"/>
-      <c r="B28" s="83" t="s">
+      <c r="B28" s="82" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="78"/>
@@ -3767,7 +3767,7 @@
     </row>
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="58"/>
-      <c r="B29" s="83" t="s">
+      <c r="B29" s="82" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="78"/>
@@ -3842,7 +3842,7 @@
     </row>
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="58"/>
-      <c r="B30" s="83" t="s">
+      <c r="B30" s="82" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="78"/>
@@ -3917,7 +3917,7 @@
     </row>
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="58"/>
-      <c r="B31" s="83" t="s">
+      <c r="B31" s="82" t="s">
         <v>2</v>
       </c>
       <c r="C31" s="78"/>
@@ -3994,7 +3994,7 @@
       <c r="A32" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="84"/>
+      <c r="B32" s="83"/>
       <c r="C32" s="79"/>
       <c r="D32" s="16"/>
       <c r="E32" s="70"/>
@@ -4146,11 +4146,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4158,6 +4153,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">

</xml_diff>

<commit_message>
updated gantt chart and read me
</commit_message>
<xml_diff>
--- a/Gant Chart.xlsx
+++ b/Gant Chart.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7691ABB9-5E1D-4141-AE6E-9F77109510FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -20,9 +19,9 @@
     <definedName name="task_start" localSheetId="0">ProjectSchedule!$E1</definedName>
     <definedName name="today" localSheetId="0">TODAY()</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>Task 3</t>
   </si>
@@ -240,9 +239,6 @@
     <t xml:space="preserve">Megha </t>
   </si>
   <si>
-    <t>Megha &amp; Dannie</t>
-  </si>
-  <si>
     <t>Building out the dbms</t>
   </si>
   <si>
@@ -261,15 +257,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="165" formatCode="ddd\,\ m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="d"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="166" formatCode="ddd\,\ m/d/yyyy"/>
+    <numFmt numFmtId="167" formatCode="mmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="168" formatCode="d"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -644,7 +640,7 @@
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="3" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
@@ -653,10 +649,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" applyFill="0">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" applyFill="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyFill="0">
@@ -693,13 +689,13 @@
     <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="11" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="11" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="11" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -719,10 +715,10 @@
     <xf numFmtId="9" fontId="5" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -734,10 +730,10 @@
     <xf numFmtId="9" fontId="5" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -749,10 +745,10 @@
     <xf numFmtId="9" fontId="5" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="11" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -764,10 +760,10 @@
     <xf numFmtId="9" fontId="5" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="10" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -782,10 +778,10 @@
     <xf numFmtId="9" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -851,19 +847,19 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="10" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="10" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="11" borderId="2" xfId="10" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="2" xfId="10" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="10">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="2" xfId="10" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="2" xfId="10" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="11" borderId="2" xfId="10" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="10" borderId="2" xfId="10" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="10">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="11" applyFill="1">
@@ -911,6 +907,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -918,33 +926,21 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Date" xfId="10" xr:uid="{229918B6-DD13-4F5A-97B9-305F7E002AA3}"/>
+    <cellStyle name="Date" xfId="10"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Name" xfId="11" xr:uid="{B2D3C1EE-6B41-4801-AAFC-C2274E49E503}"/>
+    <cellStyle name="Name" xfId="11"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="Project Start" xfId="9" xr:uid="{8EB8A09A-C31C-40A3-B2C1-9449520178B8}"/>
-    <cellStyle name="Task" xfId="12" xr:uid="{6391D789-272B-4DD2-9BF3-2CDCF610FA41}"/>
+    <cellStyle name="Project Start" xfId="9"/>
+    <cellStyle name="Task" xfId="12"/>
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
+    <cellStyle name="zHiddenText" xfId="3"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -1072,7 +1068,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="ToDoList" pivot="0" count="9">
       <tableStyleElement type="wholeTable" dxfId="11"/>
       <tableStyleElement type="headerRow" dxfId="10"/>
       <tableStyleElement type="totalRow" dxfId="9"/>
@@ -1195,7 +1191,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1207,7 +1203,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1273,7 +1269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Calibri">
       <a:majorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="メイリオ"/>
@@ -1308,7 +1304,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="メイリオ"/>
@@ -1485,44 +1481,44 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BL36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="58" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" customWidth="1"/>
     <col min="3" max="3" width="30.6640625" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
     <col min="7" max="7" width="2.6640625" customWidth="1"/>
-    <col min="8" max="8" width="6.1640625" hidden="1" customWidth="1"/>
-    <col min="9" max="64" width="2.5" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" hidden="1" customWidth="1"/>
+    <col min="9" max="64" width="2.44140625" customWidth="1"/>
     <col min="69" max="70" width="10.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" ht="30" customHeight="1">
       <c r="A1" s="59" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1533,7 +1529,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" ht="30" customHeight="1">
       <c r="A2" s="58" t="s">
         <v>33</v>
       </c>
@@ -1544,125 +1540,125 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:64" ht="30" customHeight="1">
       <c r="A3" s="58" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="E3" s="92">
+      <c r="D3" s="91"/>
+      <c r="E3" s="89">
         <f ca="1">TODAY()</f>
-        <v>43562</v>
-      </c>
-      <c r="F3" s="92"/>
-    </row>
-    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>43563</v>
+      </c>
+      <c r="F3" s="89"/>
+    </row>
+    <row r="4" spans="1:64" ht="30" customHeight="1">
       <c r="A4" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="87"/>
+      <c r="D4" s="91"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="89">
+      <c r="I4" s="86">
         <f ca="1">I5</f>
         <v>43563</v>
       </c>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="91"/>
-      <c r="P4" s="89">
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="86">
         <f ca="1">P5</f>
         <v>43570</v>
       </c>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="91"/>
-      <c r="W4" s="89">
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
+      <c r="V4" s="88"/>
+      <c r="W4" s="86">
         <f ca="1">W5</f>
         <v>43577</v>
       </c>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
-      <c r="AA4" s="90"/>
-      <c r="AB4" s="90"/>
-      <c r="AC4" s="91"/>
-      <c r="AD4" s="89">
+      <c r="X4" s="87"/>
+      <c r="Y4" s="87"/>
+      <c r="Z4" s="87"/>
+      <c r="AA4" s="87"/>
+      <c r="AB4" s="87"/>
+      <c r="AC4" s="88"/>
+      <c r="AD4" s="86">
         <f ca="1">AD5</f>
         <v>43584</v>
       </c>
-      <c r="AE4" s="90"/>
-      <c r="AF4" s="90"/>
-      <c r="AG4" s="90"/>
-      <c r="AH4" s="90"/>
-      <c r="AI4" s="90"/>
-      <c r="AJ4" s="91"/>
-      <c r="AK4" s="89">
+      <c r="AE4" s="87"/>
+      <c r="AF4" s="87"/>
+      <c r="AG4" s="87"/>
+      <c r="AH4" s="87"/>
+      <c r="AI4" s="87"/>
+      <c r="AJ4" s="88"/>
+      <c r="AK4" s="86">
         <f ca="1">AK5</f>
         <v>43591</v>
       </c>
-      <c r="AL4" s="90"/>
-      <c r="AM4" s="90"/>
-      <c r="AN4" s="90"/>
-      <c r="AO4" s="90"/>
-      <c r="AP4" s="90"/>
-      <c r="AQ4" s="91"/>
-      <c r="AR4" s="89">
+      <c r="AL4" s="87"/>
+      <c r="AM4" s="87"/>
+      <c r="AN4" s="87"/>
+      <c r="AO4" s="87"/>
+      <c r="AP4" s="87"/>
+      <c r="AQ4" s="88"/>
+      <c r="AR4" s="86">
         <f ca="1">AR5</f>
         <v>43598</v>
       </c>
-      <c r="AS4" s="90"/>
-      <c r="AT4" s="90"/>
-      <c r="AU4" s="90"/>
-      <c r="AV4" s="90"/>
-      <c r="AW4" s="90"/>
-      <c r="AX4" s="91"/>
-      <c r="AY4" s="89">
+      <c r="AS4" s="87"/>
+      <c r="AT4" s="87"/>
+      <c r="AU4" s="87"/>
+      <c r="AV4" s="87"/>
+      <c r="AW4" s="87"/>
+      <c r="AX4" s="88"/>
+      <c r="AY4" s="86">
         <f ca="1">AY5</f>
         <v>43605</v>
       </c>
-      <c r="AZ4" s="90"/>
-      <c r="BA4" s="90"/>
-      <c r="BB4" s="90"/>
-      <c r="BC4" s="90"/>
-      <c r="BD4" s="90"/>
-      <c r="BE4" s="91"/>
-      <c r="BF4" s="89">
+      <c r="AZ4" s="87"/>
+      <c r="BA4" s="87"/>
+      <c r="BB4" s="87"/>
+      <c r="BC4" s="87"/>
+      <c r="BD4" s="87"/>
+      <c r="BE4" s="88"/>
+      <c r="BF4" s="86">
         <f ca="1">BF5</f>
         <v>43612</v>
       </c>
-      <c r="BG4" s="90"/>
-      <c r="BH4" s="90"/>
-      <c r="BI4" s="90"/>
-      <c r="BJ4" s="90"/>
-      <c r="BK4" s="90"/>
-      <c r="BL4" s="91"/>
-    </row>
-    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG4" s="87"/>
+      <c r="BH4" s="87"/>
+      <c r="BI4" s="87"/>
+      <c r="BJ4" s="87"/>
+      <c r="BK4" s="87"/>
+      <c r="BL4" s="88"/>
+    </row>
+    <row r="5" spans="1:64" ht="15" customHeight="1">
       <c r="A5" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43563</v>
@@ -1888,7 +1884,7 @@
         <v>43618</v>
       </c>
     </row>
-    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1">
       <c r="A6" s="59" t="s">
         <v>43</v>
       </c>
@@ -2136,7 +2132,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1">
       <c r="A7" s="58" t="s">
         <v>38</v>
       </c>
@@ -2203,12 +2199,12 @@
       <c r="BK7" s="44"/>
       <c r="BL7" s="44"/>
     </row>
-    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A8" s="59" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="71"/>
       <c r="D8" s="19"/>
@@ -2276,22 +2272,18 @@
       <c r="BK8" s="44"/>
       <c r="BL8" s="44"/>
     </row>
-    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A9" s="59" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="84" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="22">
-        <v>0.9</v>
-      </c>
+      <c r="C9" s="84"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="66">
         <f ca="1">Project_Start</f>
-        <v>43562</v>
+        <v>43563</v>
       </c>
       <c r="F9" s="66"/>
       <c r="G9" s="17"/>
@@ -2356,7 +2348,7 @@
       <c r="BK9" s="44"/>
       <c r="BL9" s="44"/>
     </row>
-    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A10" s="59" t="s">
         <v>46</v>
       </c>
@@ -2364,18 +2356,19 @@
         <v>51</v>
       </c>
       <c r="C10" s="84" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D10" s="22">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E10" s="66">
-        <v>43551</v>
+        <f ca="1">Project_Start</f>
+        <v>43563</v>
       </c>
       <c r="F10" s="66"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="I10" s="44"/>
@@ -2435,18 +2428,20 @@
       <c r="BK10" s="44"/>
       <c r="BL10" s="44"/>
     </row>
-    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A11" s="58"/>
       <c r="B11" s="85" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="84" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" s="22">
-        <v>0</v>
-      </c>
-      <c r="E11" s="66"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="66">
+        <v>43528</v>
+      </c>
       <c r="F11" s="66"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17" t="str">
@@ -2510,13 +2505,13 @@
       <c r="BK11" s="44"/>
       <c r="BL11" s="44"/>
     </row>
-    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A12" s="58"/>
       <c r="B12" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="84" t="s">
         <v>55</v>
-      </c>
-      <c r="C12" s="84" t="s">
-        <v>56</v>
       </c>
       <c r="D12" s="22">
         <v>0</v>
@@ -2585,10 +2580,10 @@
       <c r="BK12" s="44"/>
       <c r="BL12" s="44"/>
     </row>
-    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="58"/>
       <c r="B13" s="85" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="72"/>
       <c r="D13" s="22"/>
@@ -2656,7 +2651,7 @@
       <c r="BK13" s="44"/>
       <c r="BL13" s="44"/>
     </row>
-    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A14" s="59" t="s">
         <v>47</v>
       </c>
@@ -2729,7 +2724,7 @@
       <c r="BK14" s="44"/>
       <c r="BL14" s="44"/>
     </row>
-    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A15" s="59"/>
       <c r="B15" s="80" t="s">
         <v>4</v>
@@ -2800,7 +2795,7 @@
       <c r="BK15" s="44"/>
       <c r="BL15" s="44"/>
     </row>
-    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A16" s="58"/>
       <c r="B16" s="80" t="s">
         <v>5</v>
@@ -2871,7 +2866,7 @@
       <c r="BK16" s="44"/>
       <c r="BL16" s="44"/>
     </row>
-    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A17" s="58"/>
       <c r="B17" s="80" t="s">
         <v>0</v>
@@ -2942,7 +2937,7 @@
       <c r="BK17" s="44"/>
       <c r="BL17" s="44"/>
     </row>
-    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A18" s="58"/>
       <c r="B18" s="80" t="s">
         <v>1</v>
@@ -3013,7 +3008,7 @@
       <c r="BK18" s="44"/>
       <c r="BL18" s="44"/>
     </row>
-    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A19" s="58"/>
       <c r="B19" s="80" t="s">
         <v>2</v>
@@ -3084,7 +3079,7 @@
       <c r="BK19" s="44"/>
       <c r="BL19" s="44"/>
     </row>
-    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A20" s="58" t="s">
         <v>35</v>
       </c>
@@ -3157,7 +3152,7 @@
       <c r="BK20" s="44"/>
       <c r="BL20" s="44"/>
     </row>
-    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A21" s="58"/>
       <c r="B21" s="81" t="s">
         <v>4</v>
@@ -3166,11 +3161,11 @@
       <c r="D21" s="32"/>
       <c r="E21" s="68">
         <f ca="1">E9+15</f>
-        <v>43577</v>
+        <v>43578</v>
       </c>
       <c r="F21" s="68">
         <f ca="1">E21+5</f>
-        <v>43582</v>
+        <v>43583</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17">
@@ -3234,7 +3229,7 @@
       <c r="BK21" s="44"/>
       <c r="BL21" s="44"/>
     </row>
-    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A22" s="58"/>
       <c r="B22" s="81" t="s">
         <v>5</v>
@@ -3243,11 +3238,11 @@
       <c r="D22" s="32"/>
       <c r="E22" s="68">
         <f ca="1">F21+1</f>
-        <v>43583</v>
+        <v>43584</v>
       </c>
       <c r="F22" s="68">
         <f ca="1">E22+4</f>
-        <v>43587</v>
+        <v>43588</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17">
@@ -3311,7 +3306,7 @@
       <c r="BK22" s="44"/>
       <c r="BL22" s="44"/>
     </row>
-    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A23" s="58"/>
       <c r="B23" s="81" t="s">
         <v>0</v>
@@ -3320,11 +3315,11 @@
       <c r="D23" s="32"/>
       <c r="E23" s="68">
         <f ca="1">E22+5</f>
-        <v>43588</v>
+        <v>43589</v>
       </c>
       <c r="F23" s="68">
         <f ca="1">E23+5</f>
-        <v>43593</v>
+        <v>43594</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17">
@@ -3388,7 +3383,7 @@
       <c r="BK23" s="44"/>
       <c r="BL23" s="44"/>
     </row>
-    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A24" s="58"/>
       <c r="B24" s="81" t="s">
         <v>1</v>
@@ -3397,11 +3392,11 @@
       <c r="D24" s="32"/>
       <c r="E24" s="68">
         <f ca="1">F23+1</f>
-        <v>43594</v>
+        <v>43595</v>
       </c>
       <c r="F24" s="68">
         <f ca="1">E24+4</f>
-        <v>43598</v>
+        <v>43599</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17">
@@ -3465,7 +3460,7 @@
       <c r="BK24" s="44"/>
       <c r="BL24" s="44"/>
     </row>
-    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A25" s="58"/>
       <c r="B25" s="81" t="s">
         <v>2</v>
@@ -3474,11 +3469,11 @@
       <c r="D25" s="32"/>
       <c r="E25" s="68">
         <f ca="1">E23</f>
-        <v>43588</v>
+        <v>43589</v>
       </c>
       <c r="F25" s="68">
         <f ca="1">E25+4</f>
-        <v>43592</v>
+        <v>43593</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="17">
@@ -3542,7 +3537,7 @@
       <c r="BK25" s="44"/>
       <c r="BL25" s="44"/>
     </row>
-    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A26" s="58" t="s">
         <v>35</v>
       </c>
@@ -3615,7 +3610,7 @@
       <c r="BK26" s="44"/>
       <c r="BL26" s="44"/>
     </row>
-    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A27" s="58"/>
       <c r="B27" s="82" t="s">
         <v>4</v>
@@ -3690,7 +3685,7 @@
       <c r="BK27" s="44"/>
       <c r="BL27" s="44"/>
     </row>
-    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A28" s="58"/>
       <c r="B28" s="82" t="s">
         <v>5</v>
@@ -3765,7 +3760,7 @@
       <c r="BK28" s="44"/>
       <c r="BL28" s="44"/>
     </row>
-    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A29" s="58"/>
       <c r="B29" s="82" t="s">
         <v>0</v>
@@ -3840,7 +3835,7 @@
       <c r="BK29" s="44"/>
       <c r="BL29" s="44"/>
     </row>
-    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A30" s="58"/>
       <c r="B30" s="82" t="s">
         <v>1</v>
@@ -3915,7 +3910,7 @@
       <c r="BK30" s="44"/>
       <c r="BL30" s="44"/>
     </row>
-    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A31" s="58"/>
       <c r="B31" s="82" t="s">
         <v>2</v>
@@ -3990,7 +3985,7 @@
       <c r="BK31" s="44"/>
       <c r="BL31" s="44"/>
     </row>
-    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A32" s="58" t="s">
         <v>37</v>
       </c>
@@ -4061,7 +4056,7 @@
       <c r="BK32" s="44"/>
       <c r="BL32" s="44"/>
     </row>
-    <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A33" s="59" t="s">
         <v>36</v>
       </c>
@@ -4134,18 +4129,23 @@
       <c r="BK33" s="46"/>
       <c r="BL33" s="46"/>
     </row>
-    <row r="34" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:64" ht="30" customHeight="1">
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:64" ht="30" customHeight="1">
       <c r="C35" s="14"/>
       <c r="F35" s="60"/>
     </row>
-    <row r="36" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:64" ht="30" customHeight="1">
       <c r="C36" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4153,11 +4153,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">
@@ -4187,13 +4182,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="E4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="E4">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="I1" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I1" r:id="rId2"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
@@ -4229,101 +4224,101 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="87.1640625" style="48" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="2"/>
+    <col min="1" max="1" width="87.109375" style="48" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:2" s="50" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1"/>
+    <row r="2" spans="1:2" s="50" customFormat="1" ht="15.6">
       <c r="A2" s="49" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="49"/>
     </row>
-    <row r="3" spans="1:2" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" s="54" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="55" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="55"/>
     </row>
-    <row r="4" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="51" customFormat="1" ht="25.8">
       <c r="A4" s="52" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="73.95" customHeight="1">
       <c r="A5" s="53" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1">
       <c r="A6" s="52" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="48" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" s="48" customFormat="1" ht="205.05" customHeight="1">
       <c r="A7" s="57" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" s="51" customFormat="1" ht="25.8">
       <c r="A8" s="52" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="57.6">
       <c r="A9" s="53" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="48" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" s="48" customFormat="1" ht="28.05" customHeight="1">
       <c r="A10" s="56" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" s="51" customFormat="1" ht="25.8">
       <c r="A11" s="52" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="28.8">
       <c r="A12" s="53" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="48" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" s="48" customFormat="1" ht="28.05" customHeight="1">
       <c r="A13" s="56" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" s="51" customFormat="1" ht="25.8">
       <c r="A14" s="52" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="75" customHeight="1">
       <c r="A15" s="53" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="72">
       <c r="A16" s="53" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="A2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="A13" r:id="rId1"/>
+    <hyperlink ref="A10" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>